<commit_message>
Updated report and excel sheet.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\AI Pathfinding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl Ward\Desktop\AI-Pathfinding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB0AD21C-82A9-4B09-B862-C3ABE1437EBC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846CEDC0-ADDA-432C-A92B-57A53E6D0F14}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{6164E937-4604-4378-853F-72EBE774A071}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>Release</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Generations</t>
   </si>
@@ -64,6 +58,24 @@
   </si>
   <si>
     <t>1000x1000 (Complex)</t>
+  </si>
+  <si>
+    <t>Memory Usage (MB)</t>
+  </si>
+  <si>
+    <t>Memory Processed (MB)</t>
+  </si>
+  <si>
+    <t>A* Time Taken (Debug)</t>
+  </si>
+  <si>
+    <t>A* Time Taken (Release)</t>
+  </si>
+  <si>
+    <t>Time Taken to Train (Debug)</t>
+  </si>
+  <si>
+    <t>Time Taken to Train (Release)</t>
   </si>
 </sst>
 </file>
@@ -156,7 +168,7 @@
               <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Average Time Taken to Solve (Seconds)</a:t>
+              <a:t>Time Taken to Train (Seconds)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB">
               <a:effectLst/>
@@ -209,7 +221,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Debug</c:v>
+                  <c:v>Time Taken to Train (Debug)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -310,7 +322,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Release</c:v>
+                  <c:v>Time Taken to Train (Release)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -598,7 +610,1397 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Generations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x10 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x10 (Impossible)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100x100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100x100 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100x100 (Impossible)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000x1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000x1000 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000x1000 (Impossible)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1027</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1093</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1936</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2436.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2807.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3178.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3548.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3919.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-83FD-4B9A-B111-8021554AF9BF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="591312072"/>
+        <c:axId val="591311744"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="591312072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="591311744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="591311744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="591312072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Memory</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Diagnostics (MB)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Memory Usage (MB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x10 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x10 (Impossible)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100x100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100x100 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100x100 (Impossible)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000x1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000x1000 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000x1000 (Impossible)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-66F3-49F5-BCE8-EB9E319F7AA8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Memory Processed (MB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x10 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x10 (Impossible)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100x100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100x100 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100x100 (Impossible)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000x1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000x1000 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000x1000 (Impossible)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-66F3-49F5-BCE8-EB9E319F7AA8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="591309448"/>
+        <c:axId val="591315024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="591309448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="591315024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="591315024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="591309448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>A* Time Taken (Seconds)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* Time Taken (Debug)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x10 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x10 (Impossible)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100x100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100x100 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100x100 (Impossible)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000x1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000x1000 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000x1000 (Impossible)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C983-494C-B8B7-3F98952DC573}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* Time Taken (Release)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x10 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x10 (Impossible)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100x100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100x100 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100x100 (Impossible)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000x1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000x1000 (Complex)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000x1000 (Impossible)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C983-494C-B8B7-3F98952DC573}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="585761032"/>
+        <c:axId val="585763656"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="585761032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585763656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="585763656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585761032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1141,20 +2543,1529 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>261937</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1174,6 +4085,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54E5470E-24DA-419A-A5EA-CDC5D43D72F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB173A47-25C4-45ED-8FBC-10DB89D25E34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E160A127-ED58-4626-A755-5BE5126797AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1479,10 +4498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E61490-C04E-436A-AE00-81EECE47BADF}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,23 +4509,35 @@
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="E1" t="s">
+        <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>10</v>
@@ -1514,13 +4545,25 @@
       <c r="C2" s="1">
         <v>2</v>
       </c>
+      <c r="D2">
+        <v>1027</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
       <c r="F2">
-        <v>1027</v>
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>20</v>
@@ -1528,13 +4571,25 @@
       <c r="C3" s="1">
         <v>4</v>
       </c>
+      <c r="D3">
+        <v>1093</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
       <c r="F3">
-        <v>1093</v>
+        <v>34</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>30</v>
@@ -1542,13 +4597,25 @@
       <c r="C4" s="1">
         <v>6</v>
       </c>
+      <c r="D4">
+        <v>1936</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
       <c r="F4">
-        <v>1936</v>
+        <v>39</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -1556,13 +4623,25 @@
       <c r="C5" s="1">
         <v>8</v>
       </c>
+      <c r="D5">
+        <v>1982</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
       <c r="F5">
-        <v>1982</v>
+        <v>44</v>
+      </c>
+      <c r="G5">
+        <v>40</v>
+      </c>
+      <c r="H5">
+        <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>50</v>
@@ -1570,10 +4649,25 @@
       <c r="C6" s="1">
         <v>10</v>
       </c>
+      <c r="D6">
+        <v>2436.5</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>49</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>60</v>
@@ -1581,10 +4675,25 @@
       <c r="C7" s="1">
         <v>12</v>
       </c>
+      <c r="D7">
+        <v>2807.3</v>
+      </c>
+      <c r="E7">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>54</v>
+      </c>
+      <c r="G7">
+        <v>60</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>70</v>
@@ -1592,10 +4701,25 @@
       <c r="C8" s="1">
         <v>14</v>
       </c>
+      <c r="D8">
+        <v>3178.1</v>
+      </c>
+      <c r="E8">
+        <v>26</v>
+      </c>
+      <c r="F8">
+        <v>59</v>
+      </c>
+      <c r="G8">
+        <v>70</v>
+      </c>
+      <c r="H8">
+        <v>70</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>80</v>
@@ -1603,16 +4727,46 @@
       <c r="C9" s="1">
         <v>16</v>
       </c>
+      <c r="D9">
+        <v>3548.9</v>
+      </c>
+      <c r="E9">
+        <v>29</v>
+      </c>
+      <c r="F9">
+        <v>64</v>
+      </c>
+      <c r="G9">
+        <v>80</v>
+      </c>
+      <c r="H9">
+        <v>80</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>90</v>
       </c>
       <c r="C10" s="1">
         <v>18</v>
+      </c>
+      <c r="D10">
+        <v>3919.7</v>
+      </c>
+      <c r="E10">
+        <v>32</v>
+      </c>
+      <c r="F10">
+        <v>69</v>
+      </c>
+      <c r="G10">
+        <v>90</v>
+      </c>
+      <c r="H10">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>